<commit_message>
fix: Added support for deal costs and day prices and quantities.
</commit_message>
<xml_diff>
--- a/analysis/performancetesting.xlsx
+++ b/analysis/performancetesting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\repos\dealcapture\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8EE2768-E40F-42A5-B464-11F7E727740C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7E18376-8D8E-4F13-A60C-DD20B97A6559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{829BCC8F-49CF-4B06-8596-4B77176D0EC2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Performance Project</t>
   </si>
@@ -111,6 +112,30 @@
   </si>
   <si>
     <t>Steps</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Audit and batch changes</t>
+  </si>
+  <si>
+    <t>Large volume</t>
+  </si>
+  <si>
+    <t>2 min</t>
+  </si>
+  <si>
+    <t>57 secs</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>5 sec</t>
   </si>
 </sst>
 </file>
@@ -118,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -187,19 +212,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9849AA-E857-4BD5-8995-EFE33C677EB4}">
-  <dimension ref="B2:F30"/>
+  <dimension ref="B2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -548,7 +574,7 @@
     <col min="4" max="4" width="12.1328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" s="6" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:12" s="6" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
@@ -556,12 +582,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="16.899999999999999" thickTop="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:12" ht="16.899999999999999" thickTop="1" x14ac:dyDescent="0.6">
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:12" ht="16.5" x14ac:dyDescent="0.6">
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
@@ -569,7 +595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:12" ht="16.5" x14ac:dyDescent="0.6">
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
@@ -577,7 +603,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:12" ht="16.5" x14ac:dyDescent="0.6">
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -585,18 +611,30 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="7" spans="2:12" ht="16.5" x14ac:dyDescent="0.6">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="2:5" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.6">
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="H8" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -609,8 +647,17 @@
       <c r="E9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0.3704513888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -621,7 +668,7 @@
         <v>0.3819791666666667</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -632,7 +679,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -643,7 +690,7 @@
         <v>0.3819791666666667</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>4</v>
       </c>
@@ -654,7 +701,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -665,7 +712,7 @@
         <v>0.3819791666666667</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>4</v>
       </c>
@@ -676,7 +723,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -687,7 +734,7 @@
         <v>0.3819791666666667</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>4</v>
       </c>
@@ -698,7 +745,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -709,7 +756,7 @@
         <v>0.3819791666666667</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>4</v>
       </c>
@@ -720,7 +767,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -730,16 +777,28 @@
       <c r="D20" s="2">
         <v>0.38199074074074074</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0.37048611111111113</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="2">
         <v>0.38917824074074076</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0.37248842592592596</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -752,27 +811,48 @@
       <c r="F22" s="1">
         <v>0.43124999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="12">
+        <v>0.37248842592592596</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="1">
         <v>0.43194444444444446</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="L24" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>14</v>
       </c>
       <c r="C26">
         <v>730000</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="K26" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -780,7 +860,7 @@
         <v>730000</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -788,7 +868,7 @@
         <v>730000</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>17</v>
       </c>
@@ -796,7 +876,7 @@
         <v>730000</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>13</v>
       </c>

</xml_diff>